<commit_message>
Enter data on carabid catches etc
I entered some last bit of data on carabid trap catches (from some missing vials that I found yesterday).

Also, I made a map of trap locations in QGIS and I started an R script to look into environmental variables
</commit_message>
<xml_diff>
--- a/PNR_Raw_Data/PNR2022_InvertebrateCommunity.xlsx
+++ b/PNR_Raw_Data/PNR2022_InvertebrateCommunity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/PNR_Beetles_github_folder/PNR_Raw_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2198" documentId="11_F25DC773A252ABDACC1048D9019B4AC45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A57ADCA5-D0A5-468D-8F2B-0E2728292EF6}"/>
+  <xr:revisionPtr revIDLastSave="2213" documentId="11_F25DC773A252ABDACC1048D9019B4AC45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50B6920C-83A8-4325-B22E-88CB16025882}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="20" windowWidth="19140" windowHeight="10180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="102">
   <si>
     <t>Treatment</t>
   </si>
@@ -342,6 +342,9 @@
   <si>
     <t>The datasheet lists 37 for Coleoptera and 28 for Staphylinidae. I found the rove beetle vial with the 28 Staphylinids but I cant find the beetle vial.</t>
   </si>
+  <si>
+    <t>Apparently I pinned 5 carabids but only entered 4 into the datasheet. I don’t know how this happened.</t>
+  </si>
 </sst>
 </file>
 
@@ -456,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,6 +553,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -923,10 +935,10 @@
   <dimension ref="A1:BI194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="N105" sqref="N105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2609,7 +2621,9 @@
       <c r="I30" s="31">
         <v>0</v>
       </c>
-      <c r="J30" s="31"/>
+      <c r="J30" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="K30" s="31"/>
       <c r="L30" s="32" t="s">
         <v>60</v>
@@ -5407,51 +5421,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:58" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="21">
+    <row r="87" spans="1:58" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="33">
         <v>44755</v>
       </c>
-      <c r="B87" s="21">
+      <c r="B87" s="33">
         <v>44769</v>
       </c>
-      <c r="C87" s="22" t="str">
+      <c r="C87" s="34" t="str">
         <f t="shared" si="6"/>
         <v>F(54/13)</v>
       </c>
-      <c r="D87" s="22">
+      <c r="D87" s="34">
         <v>3</v>
       </c>
-      <c r="E87" s="23" t="str">
+      <c r="E87" s="35" t="str">
         <f t="shared" si="7"/>
         <v>3_13</v>
       </c>
-      <c r="F87" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G87" s="22">
+      <c r="F87" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G87" s="34">
         <v>54</v>
       </c>
-      <c r="H87" s="22">
+      <c r="H87" s="34">
         <v>13</v>
       </c>
-      <c r="I87" s="22">
-        <v>0</v>
-      </c>
-      <c r="J87" s="22"/>
-      <c r="K87" s="22"/>
-      <c r="L87" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="M87" s="23">
+      <c r="I87" s="34">
+        <v>0</v>
+      </c>
+      <c r="J87" s="34"/>
+      <c r="K87" s="34"/>
+      <c r="L87" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="M87" s="35">
         <v>9</v>
       </c>
-      <c r="N87" s="23">
+      <c r="N87" s="35">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O87" s="23">
+        <v>9</v>
+      </c>
+      <c r="O87" s="35">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="X87" s="35">
+        <v>1</v>
+      </c>
+      <c r="Z87" s="35">
+        <v>4</v>
+      </c>
+      <c r="AN87" s="35">
+        <v>1</v>
+      </c>
+      <c r="AP87" s="35">
+        <v>1</v>
+      </c>
+      <c r="AZ87" s="35">
+        <v>1</v>
+      </c>
+      <c r="BE87" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:58" x14ac:dyDescent="0.35">
@@ -6435,51 +6467,60 @@
       </c>
       <c r="K107" s="12"/>
     </row>
-    <row r="108" spans="1:58" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="21">
+    <row r="108" spans="1:58" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="33">
         <v>44769</v>
       </c>
-      <c r="B108" s="21">
+      <c r="B108" s="33">
         <v>44784</v>
       </c>
-      <c r="C108" s="22" t="str">
+      <c r="C108" s="34" t="str">
         <f t="shared" si="10"/>
         <v>W(51/10)</v>
       </c>
-      <c r="D108" s="22">
+      <c r="D108" s="34">
         <v>4</v>
       </c>
-      <c r="E108" s="23" t="str">
+      <c r="E108" s="35" t="str">
         <f t="shared" si="11"/>
         <v>4_10</v>
       </c>
-      <c r="F108" s="22" t="s">
+      <c r="F108" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="G108" s="22">
+      <c r="G108" s="34">
         <v>51</v>
       </c>
-      <c r="H108" s="22">
+      <c r="H108" s="34">
         <v>10</v>
       </c>
-      <c r="I108" s="22">
-        <v>0</v>
-      </c>
-      <c r="J108" s="22"/>
-      <c r="K108" s="22"/>
-      <c r="L108" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="M108" s="23">
+      <c r="I108" s="34">
+        <v>0</v>
+      </c>
+      <c r="J108" s="34"/>
+      <c r="K108" s="34"/>
+      <c r="L108" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="M108" s="35">
         <v>3</v>
       </c>
-      <c r="N108" s="23">
+      <c r="N108" s="35">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="O108" s="23">
+        <v>3</v>
+      </c>
+      <c r="O108" s="35">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="AV108" s="35">
+        <v>1</v>
+      </c>
+      <c r="AZ108" s="35">
+        <v>1</v>
+      </c>
+      <c r="BF108" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:58" x14ac:dyDescent="0.35">
@@ -10886,7 +10927,7 @@
       </c>
       <c r="X194" s="4">
         <f t="shared" si="18"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Y194" s="4">
         <f t="shared" si="18"/>
@@ -10894,7 +10935,7 @@
       </c>
       <c r="Z194" s="4">
         <f t="shared" si="18"/>
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AA194" s="4">
         <f t="shared" si="18"/>
@@ -10950,7 +10991,7 @@
       </c>
       <c r="AN194" s="4">
         <f t="shared" si="18"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AO194" s="4">
         <f t="shared" si="18"/>
@@ -10958,7 +10999,7 @@
       </c>
       <c r="AP194" s="4">
         <f t="shared" si="18"/>
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AQ194" s="4">
         <f t="shared" si="18"/>
@@ -10982,7 +11023,7 @@
       </c>
       <c r="AV194" s="4">
         <f t="shared" si="18"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AW194" s="4">
         <f t="shared" si="18"/>
@@ -10998,7 +11039,7 @@
       </c>
       <c r="AZ194" s="4">
         <f t="shared" si="18"/>
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="BA194" s="4">
         <f t="shared" si="18"/>
@@ -11018,11 +11059,11 @@
       </c>
       <c r="BE194" s="4">
         <f t="shared" si="18"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BF194" s="4">
         <f t="shared" si="18"/>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BG194" s="4">
         <f t="shared" si="18"/>

</xml_diff>

<commit_message>
Enter carabid traits, enter Silphid counts
</commit_message>
<xml_diff>
--- a/PNR_Raw_Data/PNR2022_InvertebrateCommunity.xlsx
+++ b/PNR_Raw_Data/PNR2022_InvertebrateCommunity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/PNR_Beetles_github_folder/PNR_Raw_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2604" documentId="11_F25DC773A252ABDACC1048D9019B4AC45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{025B70F7-A669-44FF-A787-C2F0DEE84F57}"/>
+  <xr:revisionPtr revIDLastSave="2718" documentId="11_F25DC773A252ABDACC1048D9019B4AC45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03704521-96E9-4BCE-AE1E-369EBF3C8320}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -941,10 +941,10 @@
   <dimension ref="A1:BH193"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D166" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BF3" sqref="BF3"/>
+      <selection pane="bottomRight" activeCell="N170" sqref="N170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11634,10 +11634,10 @@
   <dimension ref="A1:S194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N185" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T102" sqref="T102"/>
+      <selection pane="bottomRight" activeCell="O193" sqref="O193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13109,10 +13109,13 @@
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N37">
         <v>1</v>
+      </c>
+      <c r="O37">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
@@ -13759,7 +13762,7 @@
       <c r="J53" s="6"/>
       <c r="L53">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M53">
         <v>2</v>
@@ -13768,7 +13771,7 @@
         <v>1</v>
       </c>
       <c r="O53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q53">
         <v>1</v>
@@ -13882,10 +13885,13 @@
       <c r="J56" s="6"/>
       <c r="L56">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N56">
         <v>1</v>
+      </c>
+      <c r="O56">
+        <v>2</v>
       </c>
       <c r="R56">
         <v>2</v>
@@ -14221,9 +14227,12 @@
       <c r="J65" s="6"/>
       <c r="L65">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N65">
+        <v>1</v>
+      </c>
+      <c r="O65">
         <v>1</v>
       </c>
     </row>
@@ -14260,7 +14269,10 @@
       <c r="J66" s="6"/>
       <c r="L66">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="O66">
+        <v>4</v>
       </c>
       <c r="Q66">
         <v>1</v>
@@ -14443,6 +14455,9 @@
       <c r="J71" s="6"/>
       <c r="L71">
         <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O71">
         <v>1</v>
       </c>
       <c r="Q71">
@@ -14556,7 +14571,10 @@
       <c r="J74" s="6"/>
       <c r="L74">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="O74">
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.35">
@@ -14958,10 +14976,13 @@
       <c r="J85" s="6"/>
       <c r="L85">
         <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="N85">
+        <v>1</v>
+      </c>
+      <c r="O85">
         <v>6</v>
-      </c>
-      <c r="N85">
-        <v>1</v>
       </c>
       <c r="Q85">
         <v>1</v>
@@ -15075,10 +15096,13 @@
       <c r="J88" s="6"/>
       <c r="L88">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N88">
         <v>1</v>
+      </c>
+      <c r="O88">
+        <v>6</v>
       </c>
       <c r="R88">
         <v>2</v>
@@ -15117,7 +15141,10 @@
       <c r="J89" s="6"/>
       <c r="L89">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="O89">
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.35">
@@ -15153,9 +15180,12 @@
       <c r="J90" s="6"/>
       <c r="L90">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N90">
+        <v>1</v>
+      </c>
+      <c r="O90">
         <v>1</v>
       </c>
     </row>
@@ -15228,7 +15258,10 @@
       <c r="J92" s="6"/>
       <c r="L92">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="O92">
+        <v>7</v>
       </c>
       <c r="Q92">
         <v>1</v>
@@ -15309,13 +15342,13 @@
       <c r="J94" s="6"/>
       <c r="L94">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N94">
         <v>7</v>
       </c>
       <c r="O94">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R94">
         <v>1</v>
@@ -15429,10 +15462,10 @@
       <c r="J97" s="6"/>
       <c r="L97">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O97">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q97">
         <v>1</v>
@@ -15474,10 +15507,13 @@
       <c r="J98" s="6"/>
       <c r="L98">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="N98">
         <v>1</v>
+      </c>
+      <c r="O98">
+        <v>10</v>
       </c>
       <c r="R98">
         <v>3</v>
@@ -15588,7 +15624,10 @@
       <c r="J101" s="6"/>
       <c r="L101">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="O101">
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.35">
@@ -15922,7 +15961,10 @@
       <c r="J109" s="6"/>
       <c r="L109">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="O109">
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.35">
@@ -15958,7 +16000,10 @@
       <c r="J110" s="6"/>
       <c r="L110">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="O110">
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.35">
@@ -15994,10 +16039,10 @@
       <c r="J111" s="6"/>
       <c r="L111">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O111">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.35">
@@ -16105,10 +16150,10 @@
       <c r="J114" s="6"/>
       <c r="L114">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O114">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.35">
@@ -16144,7 +16189,7 @@
       <c r="J115" s="6"/>
       <c r="L115">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="M115">
         <v>5</v>
@@ -16153,7 +16198,7 @@
         <v>7</v>
       </c>
       <c r="O115">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="P115">
         <v>1</v>
@@ -16267,7 +16312,10 @@
       <c r="J118" s="6"/>
       <c r="L118">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="O118">
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.35">
@@ -17556,10 +17604,13 @@
       <c r="J153" s="6"/>
       <c r="L153">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="N153">
         <v>1</v>
+      </c>
+      <c r="O153">
+        <v>5</v>
       </c>
       <c r="R153">
         <v>5</v>
@@ -17709,10 +17760,13 @@
       <c r="J157" s="6"/>
       <c r="L157">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N157">
         <v>4</v>
+      </c>
+      <c r="O157">
+        <v>10</v>
       </c>
       <c r="R157">
         <v>10</v>
@@ -17751,10 +17805,10 @@
       <c r="J158" s="6"/>
       <c r="L158">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O158">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.35">
@@ -17898,10 +17952,10 @@
       <c r="J162" s="6"/>
       <c r="L162">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O162">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.35">
@@ -17937,7 +17991,10 @@
       <c r="J163" s="6"/>
       <c r="L163">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="O163">
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.35">
@@ -17973,7 +18030,10 @@
       <c r="J164" s="6"/>
       <c r="L164">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="O164">
+        <v>11</v>
       </c>
       <c r="R164">
         <v>1</v>
@@ -18012,9 +18072,12 @@
       <c r="J165" s="6"/>
       <c r="L165">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N165">
+        <v>1</v>
+      </c>
+      <c r="O165">
         <v>1</v>
       </c>
       <c r="R165">
@@ -18090,10 +18153,13 @@
       <c r="J167" s="6"/>
       <c r="L167">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="N167">
         <v>1</v>
+      </c>
+      <c r="O167">
+        <v>4</v>
       </c>
       <c r="R167">
         <v>10</v>
@@ -18168,6 +18234,9 @@
       <c r="J169" s="6"/>
       <c r="L169">
         <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="O169">
         <v>3</v>
       </c>
       <c r="R169">
@@ -18903,10 +18972,10 @@
       </c>
       <c r="L188">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O188">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.35">
@@ -18944,7 +19013,10 @@
       </c>
       <c r="L189">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="O189">
+        <v>1</v>
       </c>
       <c r="R189">
         <v>7</v>
@@ -19111,7 +19183,7 @@
       </c>
       <c r="O194">
         <f>SUM(O2:O193)</f>
-        <v>147</v>
+        <v>302</v>
       </c>
       <c r="P194">
         <f>SUM(P2:P193)</f>

</xml_diff>

<commit_message>
Exploratory code for environm. variables
</commit_message>
<xml_diff>
--- a/PNR_Raw_Data/PNR2022_InvertebrateCommunity.xlsx
+++ b/PNR_Raw_Data/PNR2022_InvertebrateCommunity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/PNR_Beetles_github_folder/PNR_Raw_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3110" documentId="11_F25DC773A252ABDACC1048D9019B4AC45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29E8BB35-5002-4561-8989-D5D1D44D9312}"/>
+  <xr:revisionPtr revIDLastSave="3111" documentId="11_F25DC773A252ABDACC1048D9019B4AC45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A56D122-C9FF-4D48-A85C-F77A34D20098}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,9 +282,6 @@
     <t>Trichotichnus_autumnalis</t>
   </si>
   <si>
-    <t>Amarini_unkown</t>
-  </si>
-  <si>
     <t>Anisodactylus_melanopus</t>
   </si>
   <si>
@@ -452,6 +449,9 @@
   <si>
     <t>Total_pinned_Scarab_beetles</t>
   </si>
+  <si>
+    <t>Amarini_unknown</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -657,9 +657,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1025,22 +1022,22 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1053,10 +1050,10 @@
   <dimension ref="A1:BH193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AD181" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A186" sqref="A186:XFD186"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,7 +1136,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>15</v>
@@ -1157,16 +1154,16 @@
         <v>75</v>
       </c>
       <c r="P1" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="R1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>81</v>
-      </c>
-      <c r="S1" s="23" t="s">
-        <v>82</v>
       </c>
       <c r="T1" s="23" t="s">
         <v>43</v>
@@ -1202,7 +1199,7 @@
         <v>47</v>
       </c>
       <c r="AE1" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AF1" s="23" t="s">
         <v>30</v>
@@ -1214,7 +1211,7 @@
         <v>74</v>
       </c>
       <c r="AI1" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AJ1" s="23" t="s">
         <v>46</v>
@@ -1283,7 +1280,7 @@
         <v>59</v>
       </c>
       <c r="BF1" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BG1" s="24" t="s">
         <v>45</v>
@@ -1417,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="4" t="s">
@@ -1661,151 +1658,151 @@
         <v>9</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AM9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AO9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AU9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AY9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BC9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BD9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BG9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH9" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.35">
@@ -1985,155 +1982,155 @@
         <v>1</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AM13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AO13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AU13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AY13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BC13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BD13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BG13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.35">
@@ -2608,151 +2605,151 @@
         <v>9</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AM23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AO23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AU23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AY23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BC23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BD23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BG23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.35">
@@ -3088,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K30" s="17"/>
       <c r="L30" s="18" t="s">
@@ -3301,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="4" t="s">
@@ -3566,151 +3563,151 @@
         <v>9</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AM39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AO39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AU39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AY39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BC39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BD39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BG39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:60" x14ac:dyDescent="0.35">
@@ -4091,151 +4088,151 @@
         <v>9</v>
       </c>
       <c r="L47" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AM47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AO47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AU47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AY47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BC47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BD47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BG47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH47" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:60" x14ac:dyDescent="0.35">
@@ -5674,7 +5671,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K77" s="6"/>
       <c r="L77" s="4" t="s">
@@ -5768,7 +5765,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K79" s="6"/>
       <c r="L79" s="4" t="s">
@@ -6896,155 +6893,155 @@
         <v>0</v>
       </c>
       <c r="J102" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K102" s="11"/>
       <c r="L102" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AM102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AO102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AU102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AY102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BC102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BD102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BG102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:60" x14ac:dyDescent="0.35">
@@ -7295,155 +7292,155 @@
         <v>0</v>
       </c>
       <c r="J107" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K107" s="11"/>
       <c r="L107" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AD107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AE107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AM107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AO107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AP107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AQ107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AS107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AT107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AU107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AV107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AW107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AX107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AY107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BA107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BC107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BD107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BE107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BF107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BG107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BH107" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:60" x14ac:dyDescent="0.35">
@@ -11554,11 +11551,11 @@
         <v>0</v>
       </c>
       <c r="J190" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K190" s="17"/>
       <c r="L190" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N190" s="18">
         <f t="shared" si="12"/>
@@ -11797,31 +11794,31 @@
         <v>15</v>
       </c>
       <c r="K1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="23" t="s">
+      <c r="P1" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="O1" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="P1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="R1" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="33" t="s">
         <v>105</v>
-      </c>
-      <c r="R1" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="S1" s="33" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
@@ -12113,31 +12110,31 @@
         <v>9</v>
       </c>
       <c r="K9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -12280,31 +12277,31 @@
       </c>
       <c r="J13" s="11"/>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -12672,31 +12669,31 @@
         <v>9</v>
       </c>
       <c r="K23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
@@ -13300,31 +13297,31 @@
         <v>9</v>
       </c>
       <c r="K39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
@@ -13629,31 +13626,31 @@
         <v>9</v>
       </c>
       <c r="K47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
@@ -15774,31 +15771,31 @@
       </c>
       <c r="J102" s="11"/>
       <c r="K102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.35">
@@ -15977,31 +15974,31 @@
       </c>
       <c r="J107" s="11"/>
       <c r="K107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.35">
@@ -19370,17 +19367,17 @@
       <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="35" t="s">
-        <v>136</v>
+      <c r="K1" s="23" t="s">
+        <v>135</v>
       </c>
       <c r="L1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>112</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -26822,64 +26819,64 @@
         <v>15</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L1" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="U1" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="V1" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="X1" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y1" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z1" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA1" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="N1" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="O1" s="23" t="s">
+      <c r="AB1" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="P1" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="S1" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="T1" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="U1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD1" s="33" t="s">
         <v>129</v>
-      </c>
-      <c r="V1" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="W1" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="X1" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y1" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z1" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA1" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB1" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC1" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD1" s="33" t="s">
-        <v>130</v>
       </c>
       <c r="AE1" s="33"/>
       <c r="AF1" s="33"/>

</xml_diff>